<commit_message>
Phan cong phan quan ly phan quyen: Duong + Nhat
</commit_message>
<xml_diff>
--- a/Documents/Timeline.xlsx
+++ b/Documents/Timeline.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Chức năng chính</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Thiết kế template (html, css) cho frontend &amp; toàn bộ các trang của frontend</t>
   </si>
   <si>
-    <t>Tạo masterpage cho trang admin quản lý tin tức</t>
-  </si>
-  <si>
     <t>Huệ/ Trang</t>
   </si>
   <si>
@@ -145,6 +142,60 @@
   </si>
   <si>
     <t xml:space="preserve">Tạo masterpage cho trang admin </t>
+  </si>
+  <si>
+    <t>Phân quyền chung cho trang admin</t>
+  </si>
+  <si>
+    <t>Phân quyền truy cập cho user đăng nhập</t>
+  </si>
+  <si>
+    <t>Thêm, xóa (set active = false), sửa thông tin người dùng (bảng User + bảng Profile), cho phép xem log của người dùng</t>
+  </si>
+  <si>
+    <t>Quản lý User + Log + Profile</t>
+  </si>
+  <si>
+    <t>Quản lý Group, Application, Permission</t>
+  </si>
+  <si>
+    <t>Thêm, xóa (set active = false), sửa trên các bảng Group, Application, Permission</t>
+  </si>
+  <si>
+    <t>Quản lý phân quyền người dùng</t>
+  </si>
+  <si>
+    <t>Phân quyền cho user nào thuộc group nào, group nào được phép truy cập các trang và thư mục nào (InRole, InGroup, FilePermission)</t>
+  </si>
+  <si>
+    <t>Tạo masterpage cho trang frontend</t>
+  </si>
+  <si>
+    <t>Viết tất cả các lớp partial cho các entity của phần website tin tức</t>
+  </si>
+  <si>
+    <r>
+      <t>Login, log out, kiểm tra quyền truy cập khi user login, hiển thị các trang theo phân quyền theo nhóm người dùng, ghi file log (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Làm sau cùng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -154,7 +205,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +240,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -391,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -456,9 +514,6 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -476,10 +531,40 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -511,15 +596,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -529,38 +605,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -863,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:E22"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -881,133 +945,133 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="19" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="39"/>
+      <c r="C2" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
     </row>
     <row r="4" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
     </row>
     <row r="5" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="57" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
     </row>
     <row r="7" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
-      <c r="B7" s="54" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="57" t="s">
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+    </row>
+    <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+    </row>
+    <row r="10" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="39"/>
+      <c r="B10" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-    </row>
-    <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-    </row>
-    <row r="10" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
-      <c r="B10" s="22" t="s">
+      <c r="C10" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
     </row>
     <row r="11" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="61" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
+      <c r="C11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="58"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="60"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="44"/>
     </row>
     <row r="13" spans="1:6" s="12" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -1026,15 +1090,15 @@
         <v>23</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
-        <v>34</v>
+      <c r="A14" s="64" t="s">
+        <v>33</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C14" s="18">
         <v>1</v>
@@ -1042,15 +1106,15 @@
       <c r="D14" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="50">
+      <c r="F14" s="56">
         <v>40552</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
+      <c r="A15" s="65"/>
       <c r="B15" s="9" t="s">
         <v>22</v>
       </c>
@@ -1060,20 +1124,20 @@
       <c r="D15" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="50"/>
-    </row>
-    <row r="16" spans="1:6" s="37" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
+      <c r="F15" s="56"/>
+    </row>
+    <row r="16" spans="1:6" s="46" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="33" x14ac:dyDescent="0.25">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="61" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -1085,13 +1149,13 @@
       <c r="D17" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="50">
+      <c r="E17" s="27"/>
+      <c r="F17" s="56">
         <v>40787</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="9" t="s">
         <v>25</v>
       </c>
@@ -1101,15 +1165,15 @@
       <c r="D18" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="50">
+      <c r="E18" s="27"/>
+      <c r="F18" s="56">
         <v>40583</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="21">
         <v>1</v>
@@ -1117,15 +1181,15 @@
       <c r="D19" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="27">
+      <c r="E19" s="27"/>
+      <c r="F19" s="26">
         <v>40787</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="9" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C20" s="21">
         <v>1</v>
@@ -1133,280 +1197,377 @@
       <c r="D20" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="27">
+      <c r="E20" s="27"/>
+      <c r="F20" s="26">
         <v>40789</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
+      <c r="A21" s="63"/>
       <c r="B21" s="9" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C21" s="21">
         <v>1</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="27">
+        <v>27</v>
+      </c>
+      <c r="E21" s="27"/>
+      <c r="F21" s="26">
         <v>40789</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="33"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="43">
-        <v>40797</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="43"/>
+      <c r="A22" s="48"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="32"/>
+    </row>
+    <row r="23" spans="1:11" s="6" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A23" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="21">
+        <v>2</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="59">
+        <v>40886</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="48"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="32"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="43"/>
+      <c r="A25" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="52">
+        <v>40798</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="18"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
       <c r="D26" s="7"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="43"/>
-    </row>
-    <row r="27" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="52"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="58"/>
       <c r="B27" s="9"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" s="39" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-    </row>
-    <row r="29" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="44" t="s">
-        <v>32</v>
-      </c>
+      <c r="E27" s="31"/>
+      <c r="F27" s="52"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="58"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="52"/>
+    </row>
+    <row r="29" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="58"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="43">
-        <v>40797</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="45"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="43"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="45"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" s="48" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="46"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+    </row>
+    <row r="31" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="53" t="s">
+        <v>31</v>
+      </c>
       <c r="B31" s="9"/>
-      <c r="C31" s="7"/>
+      <c r="C31" s="10"/>
       <c r="D31" s="7"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="43"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="52">
+        <v>40798</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="45"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="9"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="43"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="52"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="45"/>
+      <c r="A33" s="54"/>
       <c r="B33" s="9"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="29"/>
-      <c r="F33" s="43"/>
-    </row>
-    <row r="34" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="45"/>
+      <c r="F33" s="52"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="54"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="18"/>
+      <c r="C34" s="7"/>
       <c r="D34" s="7"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="43"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="52"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
+      <c r="A35" s="54"/>
       <c r="B35" s="9"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="43"/>
-    </row>
-    <row r="36" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="38"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38"/>
-      <c r="I36" s="38"/>
-      <c r="J36" s="38"/>
-      <c r="K36" s="38"/>
-    </row>
-    <row r="37" spans="1:11" s="5" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
-        <v>33</v>
-      </c>
+      <c r="E35" s="28"/>
+      <c r="F35" s="52"/>
+    </row>
+    <row r="36" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="54"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="52"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="55"/>
       <c r="B37" s="9"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
       <c r="E37" s="31"/>
-      <c r="F37" s="26">
-        <v>40797</v>
-      </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="38"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="38"/>
-    </row>
-    <row r="39" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="36" t="s">
+      <c r="F37" s="52"/>
+    </row>
+    <row r="38" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="47"/>
+    </row>
+    <row r="39" spans="1:11" s="5" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="20">
+        <v>2</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="35">
+        <v>40798</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="1:11" s="5" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="58"/>
+      <c r="B40" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="20">
+        <v>4</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F40" s="35">
+        <v>40798</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:11" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A41" s="58"/>
+      <c r="B41" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="20">
+        <v>3</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="F41" s="35">
+        <v>40798</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="47"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="47"/>
+    </row>
+    <row r="43" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B43" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7" t="s">
+      <c r="C43" s="7"/>
+      <c r="D43" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="31"/>
-      <c r="F39" s="34"/>
-    </row>
-    <row r="40" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="14"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="15"/>
-      <c r="F40" s="24"/>
-    </row>
-    <row r="41" spans="1:11" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="14"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="15"/>
-      <c r="F41" s="24"/>
-    </row>
-    <row r="42" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="14"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="15"/>
-      <c r="F42" s="24"/>
-    </row>
-    <row r="43" spans="1:11" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="14"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="15"/>
-      <c r="F43" s="24"/>
-    </row>
-    <row r="44" spans="1:11" s="13" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E43" s="30"/>
+      <c r="F43" s="33"/>
+    </row>
+    <row r="44" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="14"/>
       <c r="C44" s="17"/>
       <c r="D44" s="15"/>
       <c r="F44" s="24"/>
     </row>
-    <row r="45" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="14"/>
       <c r="C45" s="17"/>
       <c r="D45" s="15"/>
       <c r="F45" s="24"/>
     </row>
-    <row r="46" spans="1:11" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="14"/>
       <c r="C46" s="17"/>
       <c r="D46" s="15"/>
       <c r="F46" s="24"/>
     </row>
-    <row r="47" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="14"/>
       <c r="C47" s="17"/>
       <c r="D47" s="15"/>
       <c r="F47" s="24"/>
     </row>
-    <row r="48" spans="1:11" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="13" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="14"/>
       <c r="C48" s="17"/>
       <c r="D48" s="15"/>
       <c r="F48" s="24"/>
     </row>
-    <row r="49" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="14"/>
       <c r="C49" s="17"/>
       <c r="D49" s="15"/>
-      <c r="E49" s="13"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="24"/>
+    </row>
+    <row r="50" spans="2:6" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="14"/>
       <c r="C50" s="17"/>
       <c r="D50" s="15"/>
-      <c r="E50" s="13"/>
+      <c r="F50" s="24"/>
+    </row>
+    <row r="51" spans="2:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="14"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="15"/>
+      <c r="F51" s="24"/>
+    </row>
+    <row r="52" spans="2:6" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="14"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="15"/>
+      <c r="F52" s="24"/>
+    </row>
+    <row r="53" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="14"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="13"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="14"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="31">
+    <mergeCell ref="A42:XFD42"/>
+    <mergeCell ref="A38:XFD38"/>
+    <mergeCell ref="A16:XFD16"/>
+    <mergeCell ref="A30:XFD30"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="F25:F29"/>
+    <mergeCell ref="F31:F37"/>
+    <mergeCell ref="A31:A37"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A39:A41"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:B6"/>
@@ -1423,19 +1584,6 @@
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A38:XFD38"/>
-    <mergeCell ref="A36:XFD36"/>
-    <mergeCell ref="A16:XFD16"/>
-    <mergeCell ref="A28:XFD28"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="F23:F27"/>
-    <mergeCell ref="F29:F35"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A23:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Masterpage cho trang Admin Menu ngang trên cùng, có thêm vào các menu con, nên ai cần chức năng gì thì thêm vào đó, phần nội dung của các file aspx sử dụng lại masterpage nằm trong thẻ contentPlaceHolder. D add thêm file template có html ban đầu, đểu nếu ai cần thiết lập style cho bất kỳ trang nào có thể tham khảo
</commit_message>
<xml_diff>
--- a/Documents/Timeline.xlsx
+++ b/Documents/Timeline.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>Chức năng chính</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Chia ra test theo từng chức năng</t>
-  </si>
-  <si>
-    <t>Thủy</t>
   </si>
   <si>
     <t>Time-line dự kiến</t>
@@ -539,6 +536,60 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -551,6 +602,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -565,66 +622,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -929,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -945,133 +942,133 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="19" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+    </row>
+    <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-    </row>
-    <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39" t="s">
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="40" t="s">
+      <c r="C3" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
+    </row>
+    <row r="4" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="57"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+    </row>
+    <row r="5" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="57"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+    </row>
+    <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="57"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+    </row>
+    <row r="7" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="57"/>
+      <c r="B7" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="57"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+    </row>
+    <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="57"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
-    </row>
-    <row r="4" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-    </row>
-    <row r="5" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40" t="s">
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+    </row>
+    <row r="10" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="57"/>
+      <c r="B10" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+    </row>
+    <row r="11" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="57"/>
+      <c r="B11" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-    </row>
-    <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-    </row>
-    <row r="7" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-    </row>
-    <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-    </row>
-    <row r="10" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="B10" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-    </row>
-    <row r="11" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="44"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="64"/>
     </row>
     <row r="13" spans="1:6" s="12" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -1087,18 +1084,18 @@
         <v>2</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="64" t="s">
-        <v>33</v>
+      <c r="A14" s="59" t="s">
+        <v>32</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="18">
         <v>1</v>
@@ -1107,16 +1104,16 @@
         <v>4</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="56">
+        <v>23</v>
+      </c>
+      <c r="F14" s="52">
         <v>40552</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="65"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="21">
         <v>1</v>
@@ -1125,23 +1122,23 @@
         <v>3</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="56"/>
-    </row>
-    <row r="16" spans="1:6" s="46" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
+        <v>23</v>
+      </c>
+      <c r="F15" s="52"/>
+    </row>
+    <row r="16" spans="1:6" s="39" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
     </row>
     <row r="17" spans="1:11" ht="33" x14ac:dyDescent="0.25">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="49" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="21">
         <v>1</v>
@@ -1150,14 +1147,14 @@
         <v>9</v>
       </c>
       <c r="E17" s="27"/>
-      <c r="F17" s="56">
+      <c r="F17" s="52">
         <v>40787</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="21">
         <v>1</v>
@@ -1166,14 +1163,14 @@
         <v>9</v>
       </c>
       <c r="E18" s="27"/>
-      <c r="F18" s="56">
+      <c r="F18" s="52">
         <v>40583</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="62"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="21">
         <v>1</v>
@@ -1187,15 +1184,15 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="21">
         <v>1</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E20" s="27"/>
       <c r="F20" s="26">
@@ -1203,15 +1200,15 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="63"/>
+      <c r="A21" s="51"/>
       <c r="B21" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="21">
         <v>1</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E21" s="27"/>
       <c r="F21" s="26">
@@ -1219,19 +1216,19 @@
       </c>
     </row>
     <row r="22" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
       <c r="F22" s="32"/>
     </row>
     <row r="23" spans="1:11" s="6" customFormat="1" ht="66" x14ac:dyDescent="0.25">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="C23" s="21">
         <v>2</v>
@@ -1240,160 +1237,160 @@
         <v>3</v>
       </c>
       <c r="E23" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="59">
+        <v>51</v>
+      </c>
+      <c r="F23" s="37">
         <v>40886</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
       <c r="F24" s="32"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="58" t="s">
-        <v>30</v>
+      <c r="A25" s="54" t="s">
+        <v>29</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="18"/>
       <c r="D25" s="8"/>
       <c r="E25" s="30"/>
-      <c r="F25" s="52">
+      <c r="F25" s="45">
         <v>40798</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="58"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="31"/>
-      <c r="F26" s="52"/>
+      <c r="F26" s="45"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="58"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="9"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="31"/>
-      <c r="F27" s="52"/>
+      <c r="F27" s="45"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="58"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="9"/>
       <c r="C28" s="18"/>
       <c r="D28" s="7"/>
       <c r="E28" s="31"/>
-      <c r="F28" s="52"/>
+      <c r="F28" s="45"/>
     </row>
     <row r="29" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="58"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="9"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="31"/>
-      <c r="F29" s="52"/>
+      <c r="F29" s="45"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" s="48" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="46"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
+    <row r="30" spans="1:11" s="41" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
     </row>
     <row r="31" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="53" t="s">
-        <v>31</v>
+      <c r="A31" s="46" t="s">
+        <v>30</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
       <c r="D31" s="7"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="52">
+      <c r="F31" s="45">
         <v>40798</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
+      <c r="A32" s="47"/>
       <c r="B32" s="9"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="31"/>
-      <c r="F32" s="52"/>
+      <c r="F32" s="45"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
+      <c r="A33" s="47"/>
       <c r="B33" s="9"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="29"/>
-      <c r="F33" s="52"/>
+      <c r="F33" s="45"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="54"/>
+      <c r="A34" s="47"/>
       <c r="B34" s="9"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="28"/>
-      <c r="F34" s="52"/>
+      <c r="F34" s="45"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="54"/>
+      <c r="A35" s="47"/>
       <c r="B35" s="9"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="28"/>
-      <c r="F35" s="52"/>
+      <c r="F35" s="45"/>
     </row>
     <row r="36" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="54"/>
+      <c r="A36" s="47"/>
       <c r="B36" s="9"/>
       <c r="C36" s="18"/>
       <c r="D36" s="7"/>
       <c r="E36" s="29"/>
-      <c r="F36" s="52"/>
+      <c r="F36" s="45"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="55"/>
+      <c r="A37" s="48"/>
       <c r="B37" s="9"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="31"/>
-      <c r="F37" s="52"/>
-    </row>
-    <row r="38" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="47"/>
-      <c r="K38" s="47"/>
+      <c r="F37" s="45"/>
+    </row>
+    <row r="38" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
+      <c r="K38" s="40"/>
     </row>
     <row r="39" spans="1:11" s="5" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="58" t="s">
-        <v>32</v>
+      <c r="A39" s="54" t="s">
+        <v>31</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C39" s="20">
         <v>2</v>
@@ -1402,7 +1399,7 @@
         <v>3</v>
       </c>
       <c r="E39" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F39" s="35">
         <v>40798</v>
@@ -1414,9 +1411,9 @@
       <c r="K39" s="1"/>
     </row>
     <row r="40" spans="1:11" s="5" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="58"/>
+      <c r="A40" s="54"/>
       <c r="B40" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40" s="20">
         <v>4</v>
@@ -1425,7 +1422,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F40" s="35">
         <v>40798</v>
@@ -1437,9 +1434,9 @@
       <c r="K40" s="1"/>
     </row>
     <row r="41" spans="1:11" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.25">
-      <c r="A41" s="58"/>
+      <c r="A41" s="54"/>
       <c r="B41" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="20">
         <v>3</v>
@@ -1448,7 +1445,7 @@
         <v>3</v>
       </c>
       <c r="E41" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F41" s="35">
         <v>40798</v>
@@ -1459,17 +1456,17 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="47"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
-      <c r="I42" s="47"/>
-      <c r="J42" s="47"/>
-      <c r="K42" s="47"/>
+    <row r="42" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="40"/>
+      <c r="J42" s="40"/>
+      <c r="K42" s="40"/>
     </row>
     <row r="43" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="34" t="s">
@@ -1553,21 +1550,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A42:XFD42"/>
-    <mergeCell ref="A38:XFD38"/>
-    <mergeCell ref="A16:XFD16"/>
-    <mergeCell ref="A30:XFD30"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="F25:F29"/>
-    <mergeCell ref="F31:F37"/>
-    <mergeCell ref="A31:A37"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A39:A41"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:B6"/>
@@ -1584,6 +1566,21 @@
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A42:XFD42"/>
+    <mergeCell ref="A38:XFD38"/>
+    <mergeCell ref="A16:XFD16"/>
+    <mergeCell ref="A30:XFD30"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="F25:F29"/>
+    <mergeCell ref="F31:F37"/>
+    <mergeCell ref="A31:A37"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A39:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Timeline mới được Thủy thêm vào phần của Thủy và Thịnh.
</commit_message>
<xml_diff>
--- a/Documents/Timeline.xlsx
+++ b/Documents/Timeline.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="8445"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15600" windowHeight="8445"/>
   </bookViews>
   <sheets>
     <sheet name="Phan Cong" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
   <si>
     <t>Chức năng chính</t>
   </si>
@@ -224,15 +224,33 @@
   <si>
     <t>Done</t>
   </si>
+  <si>
+    <t>Quản lý ChucVu, GiaoVien, ToChuc</t>
+  </si>
+  <si>
+    <t>Quản lý TinTuc, LoaiTin, TaiNguyen</t>
+  </si>
+  <si>
+    <t>Thủy</t>
+  </si>
+  <si>
+    <t>Thịnh</t>
+  </si>
+  <si>
+    <t>Thêm, xóa (set active = false), sửa thông tin cho bảng TinTuc, LoaiTin, TaiNguyen</t>
+  </si>
+  <si>
+    <t>Thêm, xóa (set active = false), sửa thông tin cho bảng ChucVu, GiaoVien, ToChuc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,7 +313,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -472,11 +490,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -498,9 +527,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -541,12 +567,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -572,18 +592,69 @@
     <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -605,53 +676,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,7 +783,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -777,7 +817,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -953,161 +992,161 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="41.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="10" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="45.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="21" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="18" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:6" s="17" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A1" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-    </row>
-    <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+    </row>
+    <row r="2" spans="1:6" ht="21" customHeight="1">
+      <c r="A2" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41" t="s">
+      <c r="B2" s="55"/>
+      <c r="C2" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="55"/>
-    </row>
-    <row r="4" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42" t="s">
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
+    </row>
+    <row r="4" spans="1:6" ht="31.5" customHeight="1">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-    </row>
-    <row r="5" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42" t="s">
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+    </row>
+    <row r="5" spans="1:6" ht="75" customHeight="1">
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-    </row>
-    <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="45" t="s">
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+    </row>
+    <row r="6" spans="1:6" ht="23.25" customHeight="1">
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-    </row>
-    <row r="7" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="42" t="s">
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+    </row>
+    <row r="7" spans="1:6" ht="43.5" customHeight="1">
+      <c r="A7" s="55"/>
+      <c r="B7" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="45" t="s">
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="55"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-    </row>
-    <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42" t="s">
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+    </row>
+    <row r="9" spans="1:6" ht="37.5" customHeight="1">
+      <c r="A9" s="55"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-    </row>
-    <row r="10" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="21" t="s">
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+    </row>
+    <row r="10" spans="1:6" ht="76.5" customHeight="1">
+      <c r="A10" s="55"/>
+      <c r="B10" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-    </row>
-    <row r="11" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="21" t="s">
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+    </row>
+    <row r="11" spans="1:6" ht="52.5" customHeight="1">
+      <c r="A11" s="55"/>
+      <c r="B11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="48"/>
-    </row>
-    <row r="13" spans="1:6" s="11" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="60"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="62"/>
+    </row>
+    <row r="13" spans="1:6" s="10" customFormat="1" ht="24.75" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -1116,384 +1155,400 @@
       <c r="E13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+    <row r="14" spans="1:6" ht="95.25" customHeight="1">
+      <c r="A14" s="57" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="16">
         <v>1</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="63">
+      <c r="F14" s="50">
         <v>40552</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+    <row r="15" spans="1:6" ht="66.75" customHeight="1">
+      <c r="A15" s="58"/>
       <c r="B15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="19">
         <v>1</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="63"/>
-    </row>
-    <row r="16" spans="1:6" s="50" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-    </row>
-    <row r="17" spans="1:11" ht="33" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
+      <c r="F15" s="50"/>
+    </row>
+    <row r="16" spans="1:6" s="37" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+    </row>
+    <row r="17" spans="1:11" ht="33">
+      <c r="A17" s="47" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="19">
         <v>1</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="63">
+      <c r="E17" s="25"/>
+      <c r="F17" s="50">
         <v>40787</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="61"/>
+    <row r="18" spans="1:11">
+      <c r="A18" s="48"/>
       <c r="B18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="19">
         <v>1</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="26"/>
-      <c r="F18" s="63">
+      <c r="E18" s="25"/>
+      <c r="F18" s="50">
         <v>40583</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
+    <row r="19" spans="1:11">
+      <c r="A19" s="48"/>
       <c r="B19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="19">
         <v>1</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="25">
+      <c r="E19" s="25"/>
+      <c r="F19" s="24">
         <v>40787</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="61"/>
+    <row r="20" spans="1:11">
+      <c r="A20" s="48"/>
       <c r="B20" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="19">
         <v>1</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="26"/>
-      <c r="F20" s="25">
+      <c r="E20" s="25"/>
+      <c r="F20" s="24">
         <v>40789</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="62"/>
+    <row r="21" spans="1:11">
+      <c r="A21" s="49"/>
       <c r="B21" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="19">
         <v>1</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="26"/>
-      <c r="F21" s="25">
+      <c r="E21" s="25"/>
+      <c r="F21" s="24">
         <v>40789</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="31"/>
-    </row>
-    <row r="23" spans="1:11" s="6" customFormat="1" ht="66" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
+    <row r="22" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A22" s="39"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="1:11" s="6" customFormat="1" ht="66">
+      <c r="A23" s="34" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="19">
         <v>2</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="35" t="s">
+      <c r="E23" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="36">
+      <c r="F23" s="33">
         <v>40886</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="31"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="65" t="s">
+    <row r="24" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A24" s="39"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="28"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="52" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25" s="16">
         <v>1</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="56">
+      <c r="E25" s="26"/>
+      <c r="F25" s="43">
         <v>40798</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="65"/>
+    <row r="26" spans="1:11">
+      <c r="A26" s="52"/>
       <c r="B26" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="30"/>
-      <c r="F26" s="56"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="65"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="43"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="52"/>
       <c r="B27" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="30"/>
-      <c r="F27" s="56"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="65"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="43"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="52"/>
       <c r="B28" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="17">
+      <c r="C28" s="16">
         <v>1</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="30"/>
-      <c r="F28" s="56"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="65"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="43"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="52"/>
       <c r="B29" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="56"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="65"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="43"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="52"/>
       <c r="B30" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="56"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="65"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="43"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="52"/>
       <c r="B31" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="56"/>
-    </row>
-    <row r="32" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="65"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="43"/>
+    </row>
+    <row r="32" spans="1:11" s="5" customFormat="1">
+      <c r="A32" s="52"/>
       <c r="B32" s="8" t="s">
         <v>58</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="56"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="43"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" s="52" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="51"/>
-    </row>
-    <row r="34" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="57" t="s">
+    <row r="33" spans="1:11" s="39" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A33" s="37"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+    </row>
+    <row r="34" spans="1:11" ht="23.25" customHeight="1">
+      <c r="A34" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="56">
+      <c r="B34" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="64">
+        <v>6</v>
+      </c>
+      <c r="D34" s="64" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="43">
         <v>40798</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="58"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="56"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="58"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="56"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="58"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="56"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="58"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="56"/>
-    </row>
-    <row r="39" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="58"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="56"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="59"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="56"/>
-    </row>
-    <row r="41" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="51"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="51"/>
-      <c r="I41" s="51"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="51"/>
-    </row>
-    <row r="42" spans="1:11" s="5" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="65" t="s">
+    <row r="35" spans="1:11">
+      <c r="A35" s="45"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="43"/>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="45"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="43"/>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="45"/>
+      <c r="B37" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="64">
+        <v>6</v>
+      </c>
+      <c r="D37" s="64" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" s="43"/>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="45"/>
+      <c r="B38" s="68"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="43"/>
+    </row>
+    <row r="39" spans="1:11" s="5" customFormat="1">
+      <c r="A39" s="45"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="68"/>
+      <c r="F39" s="43"/>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="46"/>
+      <c r="B40" s="69"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="43"/>
+    </row>
+    <row r="41" spans="1:11" s="37" customFormat="1">
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="38"/>
+      <c r="K41" s="38"/>
+    </row>
+    <row r="42" spans="1:11" s="5" customFormat="1" ht="49.5">
+      <c r="A42" s="52" t="s">
         <v>30</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="19">
+      <c r="C42" s="18">
         <v>2</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D42" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E42" s="35" t="s">
+      <c r="E42" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="F42" s="34">
+      <c r="F42" s="31">
         <v>40798</v>
       </c>
       <c r="G42" s="1"/>
@@ -1502,21 +1557,21 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" s="5" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="65"/>
+    <row r="43" spans="1:11" s="5" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A43" s="52"/>
       <c r="B43" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="19">
+      <c r="C43" s="18">
         <v>4</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="35" t="s">
+      <c r="E43" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F43" s="34">
+      <c r="F43" s="31">
         <v>40798</v>
       </c>
       <c r="G43" s="1"/>
@@ -1525,21 +1580,21 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.25">
-      <c r="A44" s="65"/>
+    <row r="44" spans="1:11" s="5" customFormat="1" ht="66">
+      <c r="A44" s="52"/>
       <c r="B44" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="19">
+      <c r="C44" s="18">
         <v>3</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E44" s="35" t="s">
+      <c r="E44" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="F44" s="34">
+      <c r="F44" s="31">
         <v>40798</v>
       </c>
       <c r="G44" s="1"/>
@@ -1548,20 +1603,20 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="51"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="51"/>
-      <c r="H45" s="51"/>
-      <c r="I45" s="51"/>
-      <c r="J45" s="51"/>
-      <c r="K45" s="51"/>
-    </row>
-    <row r="46" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+    <row r="45" spans="1:11" s="37" customFormat="1">
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="38"/>
+      <c r="K45" s="38"/>
+    </row>
+    <row r="46" spans="1:11" s="11" customFormat="1">
+      <c r="A46" s="30" t="s">
         <v>12</v>
       </c>
       <c r="B46" s="6" t="s">
@@ -1571,92 +1626,84 @@
       <c r="D46" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E46" s="29"/>
-      <c r="F46" s="32"/>
-    </row>
-    <row r="47" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="13"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="14"/>
-      <c r="F47" s="23"/>
-    </row>
-    <row r="48" spans="1:11" s="12" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="13"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="14"/>
-      <c r="F48" s="23"/>
-    </row>
-    <row r="49" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="13"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="14"/>
-      <c r="F49" s="23"/>
-    </row>
-    <row r="50" spans="2:6" s="12" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="13"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="14"/>
-      <c r="F50" s="23"/>
-    </row>
-    <row r="51" spans="2:6" s="12" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="13"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="14"/>
-      <c r="F51" s="23"/>
-    </row>
-    <row r="52" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="13"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="14"/>
-      <c r="F52" s="23"/>
-    </row>
-    <row r="53" spans="2:6" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="13"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="14"/>
-      <c r="F53" s="23"/>
-    </row>
-    <row r="54" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="13"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="14"/>
-      <c r="F54" s="23"/>
-    </row>
-    <row r="55" spans="2:6" s="12" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="13"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="14"/>
-      <c r="F55" s="23"/>
-    </row>
-    <row r="56" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="13"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="12"/>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="13"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="12"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="29"/>
+    </row>
+    <row r="47" spans="1:11" s="11" customFormat="1">
+      <c r="B47" s="12"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="13"/>
+      <c r="F47" s="22"/>
+    </row>
+    <row r="48" spans="1:11" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B48" s="12"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="13"/>
+      <c r="F48" s="22"/>
+    </row>
+    <row r="49" spans="2:6" s="11" customFormat="1">
+      <c r="B49" s="12"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="13"/>
+      <c r="F49" s="22"/>
+    </row>
+    <row r="50" spans="2:6" s="11" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B50" s="12"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="13"/>
+      <c r="F50" s="22"/>
+    </row>
+    <row r="51" spans="2:6" s="11" customFormat="1" ht="24.75" customHeight="1">
+      <c r="B51" s="12"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="13"/>
+      <c r="F51" s="22"/>
+    </row>
+    <row r="52" spans="2:6" s="11" customFormat="1">
+      <c r="B52" s="12"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="13"/>
+      <c r="F52" s="22"/>
+    </row>
+    <row r="53" spans="2:6" s="11" customFormat="1" ht="39" customHeight="1">
+      <c r="B53" s="12"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="13"/>
+      <c r="F53" s="22"/>
+    </row>
+    <row r="54" spans="2:6" s="11" customFormat="1">
+      <c r="B54" s="12"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="13"/>
+      <c r="F54" s="22"/>
+    </row>
+    <row r="55" spans="2:6" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B55" s="12"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="13"/>
+      <c r="F55" s="22"/>
+    </row>
+    <row r="56" spans="2:6" ht="19.5" customHeight="1">
+      <c r="B56" s="12"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="11"/>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="B57" s="12"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="A45:XFD45"/>
-    <mergeCell ref="A41:XFD41"/>
-    <mergeCell ref="A16:XFD16"/>
-    <mergeCell ref="A33:XFD33"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="F25:F32"/>
-    <mergeCell ref="F34:F40"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A42:A44"/>
+  <mergeCells count="39">
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="D37:D40"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:B6"/>
@@ -1673,6 +1720,22 @@
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A45:XFD45"/>
+    <mergeCell ref="A41:XFD41"/>
+    <mergeCell ref="A16:XFD16"/>
+    <mergeCell ref="A33:XFD33"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="F25:F32"/>
+    <mergeCell ref="F34:F40"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="B34:B36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1680,24 +1743,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Chỉnh sửa phân công chức năng
</commit_message>
<xml_diff>
--- a/Documents/Timeline.xlsx
+++ b/Documents/Timeline.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
   <si>
     <t>Chức năng chính</t>
   </si>
@@ -222,28 +222,52 @@
     <t>Huệ</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Quản lý ChucVu, GiaoVien, ToChuc</t>
-  </si>
-  <si>
-    <t>Quản lý TinTuc, LoaiTin, TaiNguyen</t>
-  </si>
-  <si>
     <t>Thủy</t>
   </si>
   <si>
-    <t>Thịnh</t>
-  </si>
-  <si>
     <t>Thêm, xóa (set active = false), sửa thông tin cho bảng TinTuc, LoaiTin, TaiNguyen</t>
   </si>
   <si>
     <t>Thêm, xóa (set active = false), sửa thông tin cho bảng ChucVu, GiaoVien, ToChuc</t>
   </si>
   <si>
-    <t>vfdsgfd</t>
+    <t>Trang</t>
+  </si>
+  <si>
+    <t>Quản lý ChucVu, ToChuc</t>
+  </si>
+  <si>
+    <t>Quản lý GiaoVien</t>
+  </si>
+  <si>
+    <t>Phân giáo viên theo chức vụ, tổ chức</t>
+  </si>
+  <si>
+    <t>Quản lý hình ảnh upload</t>
+  </si>
+  <si>
+    <t>Quản lý TinTuc, LoaiTin, LoaiTinLv1</t>
+  </si>
+  <si>
+    <t>Tạo trang quản lý cho phép upload &amp; xóa tài nguyên</t>
+  </si>
+  <si>
+    <t>Test phần Thủy</t>
+  </si>
+  <si>
+    <t>Dương, Huệ</t>
+  </si>
+  <si>
+    <t>Test phần Dương</t>
+  </si>
+  <si>
+    <t>Test phần Huệ</t>
+  </si>
+  <si>
+    <t>Test phần Nhật</t>
+  </si>
+  <si>
+    <t>Test phần Trang</t>
   </si>
 </sst>
 </file>
@@ -316,7 +340,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -429,26 +453,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -493,22 +497,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -598,25 +591,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -637,65 +657,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -998,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1016,133 +991,133 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="17" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45" t="s">
+      <c r="B2" s="54"/>
+      <c r="C2" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="59"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
     </row>
     <row r="4" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
     </row>
     <row r="5" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46" t="s">
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="49" t="s">
+      <c r="A6" s="54"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
     </row>
     <row r="7" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="46" t="s">
+      <c r="A7" s="54"/>
+      <c r="B7" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="49" t="s">
+      <c r="A8" s="54"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
     </row>
     <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46" t="s">
+      <c r="A9" s="54"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
     </row>
     <row r="10" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
     </row>
     <row r="11" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="52"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="61"/>
     </row>
     <row r="13" spans="1:6" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -1165,7 +1140,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="56" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1180,12 +1155,12 @@
       <c r="E14" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="67">
+      <c r="F14" s="49">
         <v>40552</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
+      <c r="A15" s="57"/>
       <c r="B15" s="8" t="s">
         <v>21</v>
       </c>
@@ -1198,17 +1173,17 @@
       <c r="E15" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="67"/>
-    </row>
-    <row r="16" spans="1:6" s="54" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
+      <c r="F15" s="49"/>
+    </row>
+    <row r="16" spans="1:6" s="39" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
     </row>
     <row r="17" spans="1:11" ht="33" x14ac:dyDescent="0.25">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="46" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -1221,12 +1196,12 @@
         <v>9</v>
       </c>
       <c r="E17" s="25"/>
-      <c r="F17" s="67">
+      <c r="F17" s="49">
         <v>40787</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="65"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="8" t="s">
         <v>24</v>
       </c>
@@ -1237,12 +1212,12 @@
         <v>9</v>
       </c>
       <c r="E18" s="25"/>
-      <c r="F18" s="67">
+      <c r="F18" s="49">
         <v>40583</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="65"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="8" t="s">
         <v>26</v>
       </c>
@@ -1256,12 +1231,9 @@
       <c r="F19" s="24">
         <v>40787</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="65"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="8" t="s">
         <v>39</v>
       </c>
@@ -1275,12 +1247,9 @@
       <c r="F20" s="24">
         <v>40789</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="66"/>
+      <c r="A21" s="48"/>
       <c r="B21" s="8" t="s">
         <v>48</v>
       </c>
@@ -1296,11 +1265,11 @@
       </c>
     </row>
     <row r="22" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="56"/>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
       <c r="F22" s="28"/>
     </row>
     <row r="23" spans="1:11" s="6" customFormat="1" ht="66" x14ac:dyDescent="0.25">
@@ -1324,15 +1293,15 @@
       </c>
     </row>
     <row r="24" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="56"/>
-      <c r="B24" s="68"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
       <c r="F24" s="28"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="69" t="s">
+      <c r="A25" s="51" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="6" t="s">
@@ -1345,12 +1314,12 @@
         <v>60</v>
       </c>
       <c r="E25" s="26"/>
-      <c r="F25" s="60">
+      <c r="F25" s="45">
         <v>40798</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="69"/>
+      <c r="A26" s="51"/>
       <c r="B26" s="6" t="s">
         <v>52</v>
       </c>
@@ -1361,10 +1330,10 @@
         <v>60</v>
       </c>
       <c r="E26" s="27"/>
-      <c r="F26" s="60"/>
+      <c r="F26" s="45"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="69"/>
+      <c r="A27" s="51"/>
       <c r="B27" s="8" t="s">
         <v>53</v>
       </c>
@@ -1375,10 +1344,10 @@
         <v>60</v>
       </c>
       <c r="E27" s="27"/>
-      <c r="F27" s="60"/>
+      <c r="F27" s="45"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="69"/>
+      <c r="A28" s="51"/>
       <c r="B28" s="8" t="s">
         <v>54</v>
       </c>
@@ -1389,337 +1358,409 @@
         <v>60</v>
       </c>
       <c r="E28" s="27"/>
-      <c r="F28" s="60"/>
+      <c r="F28" s="45"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="69"/>
+      <c r="A29" s="51"/>
       <c r="B29" s="8" t="s">
         <v>55</v>
       </c>
       <c r="C29" s="16"/>
-      <c r="D29" s="18"/>
+      <c r="D29" s="18" t="s">
+        <v>60</v>
+      </c>
       <c r="E29" s="27"/>
-      <c r="F29" s="60"/>
+      <c r="F29" s="45"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="69"/>
+      <c r="A30" s="51"/>
       <c r="B30" s="8" t="s">
         <v>56</v>
       </c>
       <c r="C30" s="16"/>
-      <c r="D30" s="18"/>
+      <c r="D30" s="18" t="s">
+        <v>60</v>
+      </c>
       <c r="E30" s="27"/>
-      <c r="F30" s="60"/>
+      <c r="F30" s="45"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="69"/>
+      <c r="A31" s="51"/>
       <c r="B31" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="16"/>
-      <c r="D31" s="18"/>
+      <c r="D31" s="18" t="s">
+        <v>60</v>
+      </c>
       <c r="E31" s="27"/>
-      <c r="F31" s="60"/>
+      <c r="F31" s="45"/>
     </row>
     <row r="32" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="69"/>
+      <c r="A32" s="51"/>
       <c r="B32" s="8" t="s">
         <v>58</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="D32" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="E32" s="27"/>
-      <c r="F32" s="60"/>
+      <c r="F32" s="45"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" s="56" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
-      <c r="B33" s="55"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="55"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="55"/>
-      <c r="K33" s="55"/>
+    <row r="33" spans="1:11" s="41" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="39"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
     </row>
     <row r="34" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="61" t="s">
+      <c r="A34" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="63">
+        <v>6</v>
+      </c>
+      <c r="D34" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="45">
+        <v>40798</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="51"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="45"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="51"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="45"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="51"/>
+      <c r="B37" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="63">
+        <v>1</v>
+      </c>
+      <c r="D37" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="40">
-        <v>6</v>
-      </c>
-      <c r="D34" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="E34" s="37" t="s">
+      <c r="F37" s="45"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="51"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="45"/>
+    </row>
+    <row r="39" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="51"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="63"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="45"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="51"/>
+      <c r="B40" s="55"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="45"/>
+    </row>
+    <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="51"/>
+      <c r="B41" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="F34" s="60">
+      <c r="C41" s="18">
+        <v>1</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="37"/>
+      <c r="F41" s="45">
         <v>40798</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="62"/>
-      <c r="B35" s="38"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="60"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="62"/>
-      <c r="B36" s="39"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="60"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="62"/>
-      <c r="B37" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="40">
-        <v>6</v>
-      </c>
-      <c r="D37" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="37" t="s">
+    <row r="42" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="51"/>
+      <c r="B42" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="F37" s="60"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="62"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="60"/>
-    </row>
-    <row r="39" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="62"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="60"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="63"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="60"/>
-    </row>
-    <row r="41" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="55"/>
-      <c r="C41" s="55"/>
-      <c r="D41" s="55"/>
-      <c r="E41" s="55"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="55"/>
-      <c r="K41" s="55"/>
-    </row>
-    <row r="42" spans="1:11" s="5" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="69" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>43</v>
-      </c>
       <c r="C42" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E42" s="36" t="s">
+      <c r="E42" s="37"/>
+      <c r="F42" s="45"/>
+    </row>
+    <row r="43" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="51"/>
+      <c r="B43" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="18">
+        <v>1</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="F43" s="38">
+        <v>40798</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="40"/>
+    </row>
+    <row r="45" spans="1:11" s="5" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="18">
+        <v>2</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="F42" s="31">
+      <c r="F45" s="31">
         <v>40798</v>
       </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-    </row>
-    <row r="43" spans="1:11" s="5" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="69"/>
-      <c r="B43" s="8" t="s">
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:11" s="5" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="51"/>
+      <c r="B46" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="18">
+      <c r="C46" s="18">
         <v>4</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D46" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="32" t="s">
+      <c r="E46" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F43" s="31">
+      <c r="F46" s="31">
         <v>40798</v>
       </c>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-    </row>
-    <row r="44" spans="1:11" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.25">
-      <c r="A44" s="69"/>
-      <c r="B44" s="8" t="s">
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="1:11" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A47" s="51"/>
+      <c r="B47" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="18">
+      <c r="C47" s="18">
         <v>3</v>
       </c>
-      <c r="D44" s="18" t="s">
+      <c r="D47" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E44" s="32" t="s">
+      <c r="E47" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="F44" s="31">
+      <c r="F47" s="31">
         <v>40798</v>
       </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-    </row>
-    <row r="45" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
-      <c r="K45" s="55"/>
-    </row>
-    <row r="46" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="40"/>
+      <c r="J48" s="40"/>
+      <c r="K48" s="40"/>
+    </row>
+    <row r="49" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B49" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7" t="s">
+      <c r="C49" s="7"/>
+      <c r="D49" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E46" s="26"/>
-      <c r="F46" s="29"/>
-    </row>
-    <row r="47" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="12"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="13"/>
-      <c r="F47" s="22"/>
-    </row>
-    <row r="48" spans="1:11" s="11" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="12"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="13"/>
-      <c r="F48" s="22"/>
-    </row>
-    <row r="49" spans="2:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="12"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="13"/>
-      <c r="F49" s="22"/>
-    </row>
-    <row r="50" spans="2:6" s="11" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E49" s="26"/>
+      <c r="F49" s="29"/>
+    </row>
+    <row r="50" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="B50" s="12" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C50" s="15"/>
       <c r="D50" s="13"/>
       <c r="F50" s="22"/>
     </row>
-    <row r="51" spans="2:6" s="11" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="12"/>
+    <row r="51" spans="1:6" s="11" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="C51" s="15"/>
       <c r="D51" s="13"/>
       <c r="F51" s="22"/>
     </row>
-    <row r="52" spans="2:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="12"/>
+    <row r="52" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="C52" s="15"/>
       <c r="D52" s="13"/>
       <c r="F52" s="22"/>
     </row>
-    <row r="53" spans="2:6" s="11" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="12"/>
+    <row r="53" spans="1:6" s="11" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="C53" s="15"/>
       <c r="D53" s="13"/>
       <c r="F53" s="22"/>
     </row>
-    <row r="54" spans="2:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="12"/>
+    <row r="54" spans="1:6" s="11" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="C54" s="15"/>
       <c r="D54" s="13"/>
       <c r="F54" s="22"/>
     </row>
-    <row r="55" spans="2:6" s="11" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="12"/>
       <c r="C55" s="15"/>
       <c r="D55" s="13"/>
       <c r="F55" s="22"/>
     </row>
-    <row r="56" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" s="11" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="12"/>
       <c r="C56" s="15"/>
       <c r="D56" s="13"/>
-      <c r="E56" s="11"/>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="22"/>
+    </row>
+    <row r="57" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="12"/>
       <c r="C57" s="15"/>
       <c r="D57" s="13"/>
-      <c r="E57" s="11"/>
+      <c r="F57" s="22"/>
+    </row>
+    <row r="58" spans="1:6" s="11" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="12"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="13"/>
+      <c r="F58" s="22"/>
+    </row>
+    <row r="59" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="12"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="11"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="12"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="A45:XFD45"/>
-    <mergeCell ref="A41:XFD41"/>
-    <mergeCell ref="A16:XFD16"/>
-    <mergeCell ref="A33:XFD33"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="F25:F32"/>
-    <mergeCell ref="F34:F40"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B34:B36"/>
+  <mergeCells count="40">
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="A34:A43"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="D37:D40"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:B6"/>
@@ -1736,13 +1777,21 @@
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C2:F2"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E37:E40"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="A48:XFD48"/>
+    <mergeCell ref="A44:XFD44"/>
+    <mergeCell ref="A16:XFD16"/>
+    <mergeCell ref="A33:XFD33"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="F25:F32"/>
+    <mergeCell ref="F34:F40"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="B34:B36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>